<commit_message>
done Database, sequence, class, task Management
</commit_message>
<xml_diff>
--- a/KH_HUE_T08_ClassDiagram_v1.0.xlsx
+++ b/KH_HUE_T08_ClassDiagram_v1.0.xlsx
@@ -107,171 +107,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="60" name="Picture 59"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="28575" y="771525"/>
-          <a:ext cx="2276475" cy="2971800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="61" name="Picture 60"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3057525" y="781050"/>
-          <a:ext cx="1619250" cy="2352675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="63" name="Picture 62"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3038475" y="3790950"/>
-          <a:ext cx="1657350" cy="1733550"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -313,55 +148,38 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>18057</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85143</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="5486400" y="904875"/>
-          <a:ext cx="2219325" cy="2724150"/>
+          <a:off x="609600" y="714375"/>
+          <a:ext cx="7942857" cy="4657143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -635,7 +453,7 @@
   <dimension ref="B2:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>